<commit_message>
consistency update part 2
the registration/login/update profile function wasn't working after the consistency update - so now its been fixed, but now everything php related will be lowercase (or as close as possible).
todo: fix updateprofile updated details not showing.
</commit_message>
<xml_diff>
--- a/database/Table Structure.xlsx
+++ b/database/Table Structure.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8AF45BC-1B42-405D-AF62-E60FA3E76AC7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2687C159-7970-437E-9B3C-E724FCF35009}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sales" sheetId="4" r:id="rId1"/>
@@ -137,7 +137,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,6 +149,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="7" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -174,11 +181,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -192,6 +196,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,54 +482,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95208DCD-DC93-4454-942D-03344F8EC812}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" style="5" customWidth="1"/>
     <col min="2" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" style="3" customWidth="1"/>
     <col min="5" max="7" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+      <c r="A3" s="5">
         <v>1</v>
       </c>
       <c r="B3" t="s">
@@ -530,7 +538,7 @@
       <c r="C3" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>16</v>
       </c>
       <c r="E3" t="s">
@@ -544,7 +552,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+      <c r="A4" s="5">
         <v>2</v>
       </c>
       <c r="B4" t="s">
@@ -553,7 +561,7 @@
       <c r="C4" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>16</v>
       </c>
       <c r="E4" t="s">
@@ -567,7 +575,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+      <c r="A5" s="5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
@@ -576,7 +584,7 @@
       <c r="C5" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>16</v>
       </c>
       <c r="E5" t="s">
@@ -590,7 +598,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
+      <c r="A6" s="5">
         <v>4</v>
       </c>
       <c r="B6" t="s">
@@ -599,7 +607,7 @@
       <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>255</v>
       </c>
       <c r="F6" t="s">
@@ -610,7 +618,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
+      <c r="A7" s="5">
         <v>5</v>
       </c>
       <c r="B7" t="s">
@@ -619,7 +627,7 @@
       <c r="C7" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>16</v>
       </c>
       <c r="E7" t="s">
@@ -630,7 +638,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+      <c r="A8" s="5">
         <v>6</v>
       </c>
       <c r="B8" t="s">
@@ -639,7 +647,7 @@
       <c r="C8" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>255</v>
       </c>
       <c r="E8" t="s">
@@ -663,53 +671,53 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" style="5" customWidth="1"/>
     <col min="2" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" style="3" customWidth="1"/>
     <col min="5" max="7" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+      <c r="A3" s="5">
         <v>1</v>
       </c>
       <c r="B3" t="s">
@@ -718,7 +726,7 @@
       <c r="C3" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>16</v>
       </c>
       <c r="E3" t="s">
@@ -732,7 +740,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+      <c r="A4" s="5">
         <v>2</v>
       </c>
       <c r="B4" t="s">
@@ -741,7 +749,7 @@
       <c r="C4" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>16</v>
       </c>
       <c r="E4" t="s">
@@ -755,7 +763,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+      <c r="A5" s="5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
@@ -764,7 +772,7 @@
       <c r="C5" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>16</v>
       </c>
       <c r="E5" t="s">
@@ -775,7 +783,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
+      <c r="A6" s="5">
         <v>4</v>
       </c>
       <c r="B6" t="s">
@@ -784,7 +792,7 @@
       <c r="C6" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>255</v>
       </c>
       <c r="E6" t="s">
@@ -795,7 +803,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
+      <c r="A7" s="5">
         <v>5</v>
       </c>
       <c r="B7" t="s">
@@ -804,7 +812,7 @@
       <c r="C7" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>16</v>
       </c>
       <c r="G7" t="s">
@@ -812,7 +820,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+      <c r="A8" s="5">
         <v>6</v>
       </c>
       <c r="B8" t="s">
@@ -821,7 +829,7 @@
       <c r="C8" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>16</v>
       </c>
       <c r="G8" t="s">
@@ -839,56 +847,56 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CED7CFE-163E-43BE-BE40-222257627DD6}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" style="5" customWidth="1"/>
     <col min="2" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" style="3" customWidth="1"/>
     <col min="5" max="7" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+      <c r="A3" s="5">
         <v>1</v>
       </c>
       <c r="B3" t="s">
@@ -897,7 +905,7 @@
       <c r="C3" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>16</v>
       </c>
       <c r="E3" t="s">
@@ -911,7 +919,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+      <c r="A4" s="5">
         <v>2</v>
       </c>
       <c r="B4" t="s">
@@ -920,7 +928,7 @@
       <c r="C4" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>255</v>
       </c>
       <c r="G4" t="s">
@@ -928,7 +936,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+      <c r="A5" s="5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
@@ -937,7 +945,7 @@
       <c r="C5" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>255</v>
       </c>
       <c r="G5" t="s">
@@ -945,7 +953,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
+      <c r="A6" s="5">
         <v>4</v>
       </c>
       <c r="B6" t="s">
@@ -954,7 +962,7 @@
       <c r="C6" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>16</v>
       </c>
       <c r="G6" t="s">
@@ -962,7 +970,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
+      <c r="A7" s="5">
         <v>5</v>
       </c>
       <c r="B7" t="s">
@@ -971,12 +979,15 @@
       <c r="C7" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>255</v>
       </c>
       <c r="G7" t="s">
         <v>10</v>
       </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C13" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -997,49 +1008,49 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" style="5" customWidth="1"/>
     <col min="2" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" style="3" customWidth="1"/>
     <col min="5" max="7" width="15.7109375" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+      <c r="A3" s="5">
         <v>1</v>
       </c>
       <c r="B3" t="s">
@@ -1048,7 +1059,7 @@
       <c r="C3" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>16</v>
       </c>
       <c r="E3" t="s">
@@ -1062,7 +1073,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+      <c r="A4" s="5">
         <v>2</v>
       </c>
       <c r="B4" t="s">
@@ -1071,7 +1082,7 @@
       <c r="C4" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>255</v>
       </c>
       <c r="G4" t="s">
@@ -1079,7 +1090,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+      <c r="A5" s="5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
@@ -1088,7 +1099,7 @@
       <c r="C5" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>255</v>
       </c>
       <c r="G5" t="s">
@@ -1096,7 +1107,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
+      <c r="A6" s="5">
         <v>4</v>
       </c>
       <c r="B6" t="s">
@@ -1105,7 +1116,7 @@
       <c r="C6" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>255</v>
       </c>
       <c r="G6" t="s">
@@ -1113,7 +1124,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
+      <c r="A7" s="5">
         <v>5</v>
       </c>
       <c r="B7" t="s">
@@ -1122,7 +1133,7 @@
       <c r="C7" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>255</v>
       </c>
       <c r="G7" t="s">
@@ -1130,7 +1141,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+      <c r="A8" s="5">
         <v>6</v>
       </c>
       <c r="B8" t="s">
@@ -1139,7 +1150,7 @@
       <c r="C8" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>255</v>
       </c>
       <c r="F8" t="s">
@@ -1150,7 +1161,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
+      <c r="A9" s="5">
         <v>7</v>
       </c>
       <c r="B9" t="s">
@@ -1159,7 +1170,7 @@
       <c r="C9" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>255</v>
       </c>
       <c r="G9" t="s">

</xml_diff>

<commit_message>
Commenting - Episode 1
Addition of comments in code for php and html.
Also made the password fields show astericks instead of plain text for security.
</commit_message>
<xml_diff>
--- a/database/Table Structure.xlsx
+++ b/database/Table Structure.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2687C159-7970-437E-9B3C-E724FCF35009}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7750D207-700D-4AC5-8DA9-8D282986198C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sales" sheetId="4" r:id="rId1"/>
@@ -58,15 +58,6 @@
     <t>Not NULL</t>
   </si>
   <si>
-    <t>first-name</t>
-  </si>
-  <si>
-    <t>user-ID</t>
-  </si>
-  <si>
-    <t>last-name</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
@@ -85,36 +76,15 @@
     <t>Products</t>
   </si>
   <si>
-    <t>product-ID</t>
-  </si>
-  <si>
-    <t>product-name</t>
-  </si>
-  <si>
-    <t>total-price</t>
-  </si>
-  <si>
     <t>FLOAT</t>
   </si>
   <si>
     <t>Cart</t>
   </si>
   <si>
-    <t>product-type</t>
-  </si>
-  <si>
-    <t>product-price</t>
-  </si>
-  <si>
-    <t>product-description</t>
-  </si>
-  <si>
     <t>VARCHAR</t>
   </si>
   <si>
-    <t>product-quantity</t>
-  </si>
-  <si>
     <t>FK</t>
   </si>
   <si>
@@ -124,13 +94,43 @@
     <t>Sales</t>
   </si>
   <si>
-    <t>sale-ID</t>
-  </si>
-  <si>
-    <t>sale-timestamp</t>
-  </si>
-  <si>
     <t>timestamp</t>
+  </si>
+  <si>
+    <t>saleID</t>
+  </si>
+  <si>
+    <t>productID</t>
+  </si>
+  <si>
+    <t>userID</t>
+  </si>
+  <si>
+    <t>saletimestamp</t>
+  </si>
+  <si>
+    <t>totalprice</t>
+  </si>
+  <si>
+    <t>productprice</t>
+  </si>
+  <si>
+    <t>productname</t>
+  </si>
+  <si>
+    <t>productquantity</t>
+  </si>
+  <si>
+    <t>producttype</t>
+  </si>
+  <si>
+    <t>productdescription</t>
+  </si>
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
   </si>
 </sst>
 </file>
@@ -196,10 +196,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95208DCD-DC93-4454-942D-03344F8EC812}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,15 +495,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
+      <c r="A1" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -533,10 +533,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D3" s="3">
         <v>16</v>
@@ -556,16 +556,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="3">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
         <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="3">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>30</v>
       </c>
       <c r="F4" t="s">
         <v>9</v>
@@ -579,16 +579,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D5" s="3">
         <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="F5" t="s">
         <v>9</v>
@@ -602,16 +602,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D6" s="3">
         <v>255</v>
       </c>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G6" t="s">
         <v>10</v>
@@ -622,16 +622,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D7" s="3">
         <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="G7" t="s">
         <v>10</v>
@@ -642,16 +642,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D8" s="3">
         <v>255</v>
       </c>
       <c r="E8" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="G8" t="s">
         <v>10</v>
@@ -671,7 +671,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,15 +683,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
+      <c r="A1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -721,16 +721,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="3">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
         <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="3">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>30</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
@@ -744,16 +744,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D4" s="3">
         <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="F4" t="s">
         <v>9</v>
@@ -767,16 +767,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D5" s="3">
         <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="G5" t="s">
         <v>10</v>
@@ -787,16 +787,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D6" s="3">
         <v>255</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="G6" t="s">
         <v>10</v>
@@ -807,10 +807,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D7" s="3">
         <v>16</v>
@@ -824,10 +824,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D8" s="3">
         <v>16</v>
@@ -850,7 +850,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -862,15 +862,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
+      <c r="A1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -900,10 +900,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D3" s="3">
         <v>16</v>
@@ -923,10 +923,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D4" s="3">
         <v>255</v>
@@ -940,10 +940,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D5" s="3">
         <v>255</v>
@@ -957,10 +957,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D6" s="3">
         <v>16</v>
@@ -974,10 +974,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D7" s="3">
         <v>255</v>
@@ -987,7 +987,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C13" s="7"/>
+      <c r="C13" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1002,8 +1002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1016,15 +1016,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -1054,10 +1054,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D3" s="3">
         <v>16</v>
@@ -1077,10 +1077,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D4" s="3">
         <v>255</v>
@@ -1094,10 +1094,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D5" s="3">
         <v>255</v>
@@ -1111,10 +1111,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D6" s="3">
         <v>255</v>
@@ -1128,10 +1128,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D7" s="3">
         <v>255</v>
@@ -1145,16 +1145,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D8" s="3">
         <v>255</v>
       </c>
       <c r="F8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G8" t="s">
         <v>10</v>
@@ -1165,10 +1165,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D9" s="3">
         <v>255</v>

</xml_diff>

<commit_message>
Minor fix, database plan update
Database plan was outdated, thus it was replaced by a newer one to better reflect what the database will actually look like.
Removing html doctype messed up banner image sizing, thus i adjusted the image size to fix the problem (for now).
</commit_message>
<xml_diff>
--- a/database/Table Structure.xlsx
+++ b/database/Table Structure.xlsx
@@ -3,15 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7750D207-700D-4AC5-8DA9-8D282986198C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{893D78D3-3C99-416C-93E4-F20B85D83E0E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sales" sheetId="4" r:id="rId1"/>
-    <sheet name="Cart" sheetId="3" r:id="rId2"/>
-    <sheet name="Products" sheetId="2" r:id="rId3"/>
-    <sheet name="Users" sheetId="1" r:id="rId4"/>
+    <sheet name="Cart" sheetId="3" r:id="rId1"/>
+    <sheet name="Products" sheetId="2" r:id="rId2"/>
+    <sheet name="Users" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="33">
   <si>
     <t>Users</t>
   </si>
@@ -91,22 +90,13 @@
     <t>SMALLINT</t>
   </si>
   <si>
-    <t>Sales</t>
-  </si>
-  <si>
     <t>timestamp</t>
   </si>
   <si>
-    <t>saleID</t>
-  </si>
-  <si>
     <t>productID</t>
   </si>
   <si>
     <t>userID</t>
-  </si>
-  <si>
-    <t>saletimestamp</t>
   </si>
   <si>
     <t>totalprice</t>
@@ -479,198 +469,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95208DCD-DC93-4454-942D-03344F8EC812}">
-  <dimension ref="A1:G8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="4.28515625" style="5" customWidth="1"/>
-    <col min="2" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="3" customWidth="1"/>
-    <col min="5" max="7" width="15.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="3">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="3">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="3">
-        <v>16</v>
-      </c>
-      <c r="E5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="3">
-        <v>255</v>
-      </c>
-      <c r="F6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="3">
-        <v>16</v>
-      </c>
-      <c r="E7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="3">
-        <v>255</v>
-      </c>
-      <c r="E8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{437757BF-1C68-458C-92FB-57F7127A8EDC}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -721,7 +523,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
         <v>21</v>
@@ -744,7 +546,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
         <v>21</v>
@@ -767,7 +569,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
         <v>17</v>
@@ -787,7 +589,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
         <v>19</v>
@@ -807,7 +609,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
         <v>21</v>
@@ -824,7 +626,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
         <v>17</v>
@@ -845,7 +647,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CED7CFE-163E-43BE-BE40-222257627DD6}">
   <dimension ref="A1:G13"/>
   <sheetViews>
@@ -900,7 +702,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
         <v>21</v>
@@ -923,7 +725,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
         <v>19</v>
@@ -940,7 +742,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
         <v>19</v>
@@ -957,7 +759,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
         <v>17</v>
@@ -974,7 +776,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
@@ -998,11 +800,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -1054,7 +856,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
         <v>21</v>
@@ -1077,7 +879,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
         <v>19</v>
@@ -1094,7 +896,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
         <v>19</v>
@@ -1145,7 +947,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Setting up the code required for cart
Added an "add to cart" button to each of the products. I think it needs a little bit of tweaking to make it look better.
Also theres the database log now.
</commit_message>
<xml_diff>
--- a/database/Table Structure.xlsx
+++ b/database/Table Structure.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{893D78D3-3C99-416C-93E4-F20B85D83E0E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F4CF20-5107-4E2D-9454-628E4C5D453B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cart" sheetId="3" r:id="rId1"/>
     <sheet name="Products" sheetId="2" r:id="rId2"/>
     <sheet name="Users" sheetId="1" r:id="rId3"/>
+    <sheet name="Product Items" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="62">
   <si>
     <t>Users</t>
   </si>
@@ -121,12 +122,102 @@
   </si>
   <si>
     <t>lastname</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Jar</t>
+  </si>
+  <si>
+    <t>A small jar of oxygen. It's cute and fun!</t>
+  </si>
+  <si>
+    <t>Pristine jar of oxygen packed in a tight jar.</t>
+  </si>
+  <si>
+    <t>Large O2 Jar will last the addicted for seconds!</t>
+  </si>
+  <si>
+    <t>Jumbo O2Jar</t>
+  </si>
+  <si>
+    <t>Jumbo sized jar for a jumbo sized family.</t>
+  </si>
+  <si>
+    <t>Small O2Box</t>
+  </si>
+  <si>
+    <t>Box</t>
+  </si>
+  <si>
+    <t>Child sized box with oxygen!</t>
+  </si>
+  <si>
+    <t>Medium O2Box</t>
+  </si>
+  <si>
+    <t>Small O2Jar</t>
+  </si>
+  <si>
+    <t>Medium O2Jar</t>
+  </si>
+  <si>
+    <t>Large O2Jar</t>
+  </si>
+  <si>
+    <t>Medium sized box of oxygen is oxyllerating!</t>
+  </si>
+  <si>
+    <t>Large O2Box</t>
+  </si>
+  <si>
+    <t>Large O2Box is the perfect birthday present.</t>
+  </si>
+  <si>
+    <t>Extra Large O2Box</t>
+  </si>
+  <si>
+    <t>Big enough to fit 4 people inside!</t>
+  </si>
+  <si>
+    <t>O2Mask</t>
+  </si>
+  <si>
+    <t>Mask</t>
+  </si>
+  <si>
+    <t>O2Mask X</t>
+  </si>
+  <si>
+    <t>O2Tank</t>
+  </si>
+  <si>
+    <t>O2Backpack</t>
+  </si>
+  <si>
+    <t>Tank</t>
+  </si>
+  <si>
+    <t>Lifestyle</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -171,7 +262,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -187,6 +278,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -472,7 +564,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{437757BF-1C68-458C-92FB-57F7127A8EDC}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -485,15 +577,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -652,7 +744,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="B3" sqref="B3:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,15 +756,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -818,15 +910,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -986,4 +1078,197 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A26AF5F5-7A3B-4FD3-B6F2-3068539579F9}">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="7">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="D2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="7">
+        <v>49.99</v>
+      </c>
+      <c r="D3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="7">
+        <v>99.99</v>
+      </c>
+      <c r="D4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="7">
+        <v>169.69</v>
+      </c>
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="7">
+        <v>99.99</v>
+      </c>
+      <c r="D6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="7">
+        <v>199.99</v>
+      </c>
+      <c r="D7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="7">
+        <v>299.99</v>
+      </c>
+      <c r="D8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="7">
+        <v>449.99</v>
+      </c>
+      <c r="D9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="7">
+        <v>49.99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="7">
+        <v>999.99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="7">
+        <v>149.99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="7">
+        <v>454.49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Changes due to DB testing
Max length of each input was changed from 255 to 128 as I feel as the old max number was inappropriate and was too large. This change can be seen on the pages with input.
New SQL file to reflect this change as well.
Flowchart was updated as it forgot a crucial piece of detail: connection script.
</commit_message>
<xml_diff>
--- a/database/Table Structure.xlsx
+++ b/database/Table Structure.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A6F5B7D-A104-4246-B0EC-B313F1D3C3B7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D05FDA3C-633A-44FE-A657-E3897C3FAD1D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cart" sheetId="3" state="hidden" r:id="rId1"/>
@@ -716,8 +716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CED7CFE-163E-43BE-BE40-222257627DD6}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -796,7 +796,7 @@
         <v>19</v>
       </c>
       <c r="D4" s="3">
-        <v>255</v>
+        <v>128</v>
       </c>
       <c r="G4" t="s">
         <v>10</v>
@@ -813,7 +813,7 @@
         <v>19</v>
       </c>
       <c r="D5" s="3">
-        <v>255</v>
+        <v>128</v>
       </c>
       <c r="G5" t="s">
         <v>10</v>
@@ -829,9 +829,6 @@
       <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="3">
-        <v>16</v>
-      </c>
       <c r="G6" t="s">
         <v>10</v>
       </c>
@@ -847,7 +844,7 @@
         <v>19</v>
       </c>
       <c r="D7" s="3">
-        <v>255</v>
+        <v>128</v>
       </c>
       <c r="G7" t="s">
         <v>10</v>
@@ -869,8 +866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -950,7 +947,7 @@
         <v>19</v>
       </c>
       <c r="D4" s="3">
-        <v>255</v>
+        <v>128</v>
       </c>
       <c r="G4" t="s">
         <v>10</v>
@@ -967,7 +964,7 @@
         <v>19</v>
       </c>
       <c r="D5" s="3">
-        <v>255</v>
+        <v>128</v>
       </c>
       <c r="G5" t="s">
         <v>10</v>
@@ -984,7 +981,7 @@
         <v>19</v>
       </c>
       <c r="D6" s="3">
-        <v>255</v>
+        <v>128</v>
       </c>
       <c r="G6" t="s">
         <v>10</v>
@@ -1001,7 +998,7 @@
         <v>19</v>
       </c>
       <c r="D7" s="3">
-        <v>255</v>
+        <v>128</v>
       </c>
       <c r="G7" t="s">
         <v>10</v>
@@ -1018,7 +1015,7 @@
         <v>14</v>
       </c>
       <c r="D8" s="3">
-        <v>255</v>
+        <v>128</v>
       </c>
       <c r="F8" t="s">
         <v>15</v>
@@ -1038,7 +1035,7 @@
         <v>19</v>
       </c>
       <c r="D9" s="3">
-        <v>255</v>
+        <v>128</v>
       </c>
       <c r="G9" t="s">
         <v>10</v>

</xml_diff>